<commit_message>
fix: row with all values set to null in xls file
</commit_message>
<xml_diff>
--- a/plugins/db-wakamiti-plugin/src/test/resources/data1.xlsx
+++ b/plugins/db-wakamiti-plugin/src/test/resources/data1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo\iti\wakamiti\repo\plugins\db-wakamiti-plugin\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0281F17E-65A9-4D7B-93A5-4ECF8A50BF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3833F-C648-4A85-85E3-EF276E0F386F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30255" yWindow="2880" windowWidth="21630" windowHeight="11250" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>first_name</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>cityId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -132,9 +135,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -172,7 +175,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -278,7 +281,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -420,7 +423,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -469,6 +472,11 @@
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: datetime timezone issues
</commit_message>
<xml_diff>
--- a/plugins/db-wakamiti-plugin/src/test/resources/data1.xlsx
+++ b/plugins/db-wakamiti-plugin/src/test/resources/data1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo\iti\wakamiti\repo\plugins\db-wakamiti-plugin\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgalbis\Proyectos\temp\plugins\db-wakamiti-plugin\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3833F-C648-4A85-85E3-EF276E0F386F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E9C029-8720-4075-A472-4AB7BA4AC006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30255" yWindow="2880" windowWidth="21630" windowHeight="11250" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>first_name</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>creation</t>
+  </si>
+  <si>
+    <t>2024-07-22 12:34:56</t>
   </si>
 </sst>
 </file>
@@ -110,13 +116,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -443,10 +450,11 @@
     <col min="2" max="2" width="12.33203125"/>
     <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="1024" width="8.5546875"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="1024" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,8 +467,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -473,8 +484,11 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
fix(database): Boolean columns issues
</commit_message>
<xml_diff>
--- a/plugins/db-wakamiti-plugin/src/test/resources/data1.xlsx
+++ b/plugins/db-wakamiti-plugin/src/test/resources/data1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgalbis\Proyectos\temp\plugins\db-wakamiti-plugin\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E9C029-8720-4075-A472-4AB7BA4AC006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6585D952-B8AF-4C6E-91E2-91F49B0C8D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30255" yWindow="2880" windowWidth="21630" windowHeight="11250" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>first_name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>2024-07-22 12:34:56</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -478,8 +481,8 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>

</xml_diff>